<commit_message>
[verif] Added core scrb
</commit_message>
<xml_diff>
--- a/doc/selen/core_check_dia.xlsx
+++ b/doc/selen/core_check_dia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>IF</t>
   </si>
@@ -42,9 +42,6 @@
     <t>t2</t>
   </si>
   <si>
-    <t>core req, check=0</t>
-  </si>
-  <si>
     <t>I0</t>
   </si>
   <si>
@@ -75,33 +72,12 @@
     <t>I3</t>
   </si>
   <si>
-    <t>I0, model::execute(I0),  activate check</t>
-  </si>
-  <si>
-    <t>I1, model::execute(I1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">core req, check=1, check state after I0, model::get_reg </t>
-  </si>
-  <si>
-    <t>I2, model::execute(I2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">core req, check=1, check state after I1, model::get_reg </t>
-  </si>
-  <si>
     <t>t6</t>
   </si>
   <si>
     <t>t7</t>
   </si>
   <si>
-    <t>I3, model::execute(I3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">core req, check=1, check state after I2, model::get_reg </t>
-  </si>
-  <si>
     <t>t8</t>
   </si>
   <si>
@@ -109,6 +85,18 @@
   </si>
   <si>
     <t>* нужно проверить адрес и данные</t>
+  </si>
+  <si>
+    <t>I0, model::execute(I0), check=0 -&gt;  activate check</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check state after I0, model::get_reg , I1, model::execute(I1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check state after I1, I2, model::execute(I2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check state after I2, I3, model::execute(I3)</t>
   </si>
 </sst>
 </file>
@@ -175,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -185,6 +173,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -482,12 +475,12 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -529,10 +522,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -543,116 +536,111 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="45">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45">
       <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="1"/>
     </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="9"/>
+    </row>
     <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>